<commit_message>
Fix error in classes v1.1
</commit_message>
<xml_diff>
--- a/class_definitions/seabee_habitat_classes_v1-1.xlsx
+++ b/class_definitions/seabee_habitat_classes_v1-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HGU\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA36592-0BD8-463A-A052-3F43CF10C49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364F3E3C-01F4-44FF-A70E-CBF853B2E174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20640" yWindow="0" windowWidth="20640" windowHeight="16680" xr2:uid="{F20C8459-8D03-4AD5-899D-CF1C3A5654CA}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{F20C8459-8D03-4AD5-899D-CF1C3A5654CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1548,7 +1548,7 @@
     <xf numFmtId="0" fontId="3" fillId="69" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1899,9 +1899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{153163F2-6D79-4AA3-A08D-70B6A200403F}">
   <dimension ref="A1:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1937,7 +1935,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="80" t="s">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
@@ -3254,8 +3252,8 @@
       <c r="B59" t="s">
         <v>176</v>
       </c>
-      <c r="C59" t="s">
-        <v>97</v>
+      <c r="C59" s="80" t="s">
+        <v>176</v>
       </c>
       <c r="D59" t="s">
         <v>217</v>
@@ -3414,6 +3412,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004151AA027B066B4998584463A83F4063" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a2982693e5042b08c30196a7fc816e0d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dc71d4a8-bf34-464a-9495-9463c74aec10" xmlns:ns3="bb52825a-94a1-46f8-82cc-5d723ece883a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ace0a33c1b583bb1c0413be247d29f60" ns2:_="" ns3:_="">
     <xsd:import namespace="dc71d4a8-bf34-464a-9495-9463c74aec10"/>
@@ -3668,15 +3675,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3689,6 +3687,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76B3B49F-E441-456E-A3CC-DF2BCC4A1770}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{690F9C9D-F6E9-4EC6-B6B0-65E246495780}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3707,14 +3713,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76B3B49F-E441-456E-A3CC-DF2BCC4A1770}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B1930C17-75A8-46BE-9D01-3443FDC5646B}">
   <ds:schemaRefs>

</xml_diff>